<commit_message>
created database configurations with knex and started working on the user model
</commit_message>
<xml_diff>
--- a/server/data/sample_data.xlsx
+++ b/server/data/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\Documents\Lambda\git\prayer-room\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4876E08-30EA-4F7E-B8D2-0CB7D84EB0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58F444B-05CE-48E1-BF48-B92EF5828D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="6060" windowWidth="23256" windowHeight="12576" xr2:uid="{E7A985AE-453E-4522-AA88-5894DA5E0A44}"/>
   </bookViews>
@@ -297,24 +297,24 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,42 +663,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="14" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14" t="s">
+      <c r="N1" s="20"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="20"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="14" t="s">
+      <c r="T1" s="19"/>
+      <c r="U1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="15"/>
+      <c r="V1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -755,7 +755,7 @@
       <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="T2" s="3" t="s">
@@ -821,7 +821,7 @@
       <c r="R3" s="10">
         <v>1</v>
       </c>
-      <c r="S3" s="19">
+      <c r="S3" s="15">
         <v>1</v>
       </c>
       <c r="T3" s="7">
@@ -884,10 +884,10 @@
       <c r="Q4" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="16">
-        <v>2</v>
-      </c>
-      <c r="S4" s="20">
+      <c r="R4" s="12">
+        <v>2</v>
+      </c>
+      <c r="S4" s="16">
         <v>3</v>
       </c>
       <c r="T4" s="7">
@@ -944,10 +944,10 @@
       <c r="Q5" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="16">
-        <v>2</v>
-      </c>
-      <c r="S5" s="20">
+      <c r="R5" s="12">
+        <v>2</v>
+      </c>
+      <c r="S5" s="16">
         <v>4</v>
       </c>
       <c r="T5" s="7">
@@ -1005,10 +1005,10 @@
       <c r="R6" s="10">
         <v>1</v>
       </c>
-      <c r="S6" s="21">
-        <v>2</v>
-      </c>
-      <c r="T6" s="17">
+      <c r="S6" s="17">
+        <v>2</v>
+      </c>
+      <c r="T6" s="13">
         <v>3</v>
       </c>
       <c r="U6" s="10">
@@ -1061,13 +1061,13 @@
       <c r="Q7" t="s">
         <v>45</v>
       </c>
-      <c r="R7" s="16">
-        <v>2</v>
-      </c>
-      <c r="S7" s="21">
+      <c r="R7" s="12">
+        <v>2</v>
+      </c>
+      <c r="S7" s="17">
         <v>6</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="13">
         <v>5</v>
       </c>
       <c r="U7" s="10">
@@ -1102,8 +1102,8 @@
       <c r="L8" s="7">
         <v>1</v>
       </c>
-      <c r="R8" s="16"/>
-      <c r="S8" s="21">
+      <c r="R8" s="12"/>
+      <c r="S8" s="17">
         <v>5</v>
       </c>
       <c r="T8" s="1">

</xml_diff>